<commit_message>
Springer API calls + Fixed multiple SMILES bug
</commit_message>
<xml_diff>
--- a/Excel_Files/PubMed_Searches.xlsx
+++ b/Excel_Files/PubMed_Searches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jogeo\Desktop\Project\Blood-Brain-Barrier-Drug-Prediction\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0174FB-66CF-4A89-9ABF-4F3760EB4B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCB119B-3EA0-41EF-8863-D059D3589F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="125">
   <si>
     <t>PMID</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Database</t>
   </si>
   <si>
+    <t>Query</t>
+  </si>
+  <si>
     <t>Regular_Expression</t>
   </si>
   <si>
@@ -52,115 +55,121 @@
     <t>Class</t>
   </si>
   <si>
+    <t>https://doi.org/10.2147/IJN.S170564</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/15736415/</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/toxins12050291</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/s0161-6420(88)33038-1</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ejps.2018.03.030</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1021/acschemneuro.7b00097</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.actbio.2016.09.010</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/brain/aww096</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1113/JP271584</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.neuropharm.2015.06.010</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1172/JCI119832</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1021/mp500258p</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/17948/</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/1056-8727(92)90057-r</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2144/000114064</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1021/cn300210g</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ejmech.2012.09.035</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1124/dmd.111.042903</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1124/dmd.111.038349</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/0166-4328(94)00125-y</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3109/10611860108995630</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ijpharm.2004.10.007</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jconrel.2015.01.025</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/s0028-3908(03)00171-0</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/s0278-5846(03)00048-4</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s12640-014-9464-1</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.171325998</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/10611860410001701706</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2967/jnumed.107.047308</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1476-5381.1996.tb15160.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/ijms22147387</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1128/AAC.34.7.1360</t>
+  </si>
+  <si>
     <t>https://doi.org/10.3390/pharmaceutics13081126</t>
   </si>
   <si>
-    <t>https://doi.org/10.3390/ijms22147387</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.3390/toxins12050291</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.2147/IJN.S170564</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.ejps.2018.03.030</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1021/acschemneuro.7b00097</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.actbio.2016.09.010</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1093/brain/aww096</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1113/JP271584</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.neuropharm.2015.06.010</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.jconrel.2015.01.025</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1021/mp500258p</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/s12640-014-9464-1</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.2144/000114064</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1021/cn300210g</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.ejmech.2012.09.035</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1124/dmd.111.042903</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1124/dmd.111.038349</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.2967/jnumed.107.047308</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/15736415/</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.ijpharm.2004.10.007</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1080/10611860410001701706</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/s0028-3908(03)00171-0</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/s0278-5846(03)00048-4</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1073/pnas.171325998</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.3109/10611860108995630</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1172/JCI119832</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1111/j.1476-5381.1996.tb15160.x</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/0166-4328(94)00125-y</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/1056-8727(92)90057-r</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1128/AAC.34.7.1360</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/s0161-6420(88)33038-1</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/17948/</t>
-  </si>
-  <si>
     <t>pubmed</t>
   </si>
   <si>
+    <t>blood brain barrier permeability</t>
+  </si>
+  <si>
+    <t>.*does not cross the blood.brain barrier.*</t>
+  </si>
+  <si>
     <t>.*inability to cross the blood.brain barrier.*</t>
   </si>
   <si>
     <t>.*unable to cross the blood.brain barrier.*</t>
   </si>
   <si>
-    <t>.*does not cross the blood.brain barrier.*</t>
+    <t>.*was not able to cross the blood.brain barrier.*</t>
   </si>
   <si>
     <t>.*does not penetrate the blood.brain barrier.*</t>
@@ -169,238 +178,226 @@
     <t>.*unable to penetrate the blood.brain barrier.*</t>
   </si>
   <si>
-    <t>.*was not able to cross the blood.brain barrier.*</t>
+    <t xml:space="preserve"> 3BP does not cross the blood-brain barrier and cannot treat nervous system tumors</t>
+  </si>
+  <si>
+    <t>Despite its inability to cross the blood-brain barrier, amifostine appears promising because it protects blood vessels against radiation-induced damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> However, being unable to cross the blood-brain barrier (BBB), CNF1 requires injection directly into the brain, which is a very invasive administration route</t>
+  </si>
+  <si>
+    <t>Apraclonidine hydrochloride (ALO 2145), a clonidine derivative that does not cross the blood-brain barrier, was applied topically to one eye of each of 20 normal human subjects</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Many of the current therapeutics have limited activity due to their inability to cross the blood brain barrier which retards drug accumulation in tumor site and causes drug resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> However, their clinical usage is hindered by their inability to cross the blood-brain barrier and their poor in vivo activity after peripheral injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Although metal chelators can block these effects, their therapeutic potential is marred by their inability to cross the blood-brain barrier (BBB) and by their non-specific interactions with metal ions necessary for normal cellular processes, which could result in adverse side effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> We conclude that (11)C-dihydroergotamine is unable to cross the blood-brain barrier interictally or ictally demonstrating that the blood-brain barrier remains tight for dihydroergotamine during acute glyceryl trinitrate-induced migraine attacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Due to its hydrophilic actions, circulating AngII does not cross the blood-brain barrier (BBB), signalling to the brain via the circumventricular organs which lack a tight BBB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> However, the clinical usage of these peptides is limited because of their diminished analgesic effect following systemic injection and their inability to cross the blood-brain barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ascorbic acid was not able to cross the blood-brain barrier in our studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enzyme replacement therapy with recombinant SGSH does not treat the brain because the enzyme is a large molecule drug that does not cross the blood-brain barrier (BBB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aspartic acid, which is also considered to be a transmitter, equally does not cross the blood-brain barrier in the rat with ease</t>
+  </si>
+  <si>
+    <t>We examined the potential of astemizole, a histamine H1-receptor antagonist that does not cross the blood-brain barrier, to reverse blood-retinal barrier leakage to albumin in streptozotocin diabetic rats</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Agents unable to cross the blood brain barrier can be directly infused into the brain parenchyma or lateral ventricle through implanted cannulas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> However, MKT-077 does not penetrate the blood-brain barrier (BBB), limiting its use as either a clinical candidate or probe for exploring Hsp70 as a drug target in the central nervous system (CNS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> They showed very low permeability through (MDCK-MDR1) cells and might, therefore, represent possible lead structures for further optimization in the search for cannabinoid ligands unable to cross the blood-brain barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MPS-II affects the brain, and enzyme replacement therapy is not effective in the brain, because the enzyme does not cross the blood-brain barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> However, GDNF does not cross the blood-brain barrier (BBB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As carbachol does not cross the blood-brain barrier (BBB) due to its polar structure the data support the view that grafts of fetal neuronal tissue may induce a prolonged permeability of the BBB over a long period of time which could also be shown by HRP-histochemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> On the other hand, both DCKA and DCKA conjugates have a low brain-to-plasma concentration ratio due to their inability to cross the blood-brain barrier (BBB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Under our experimental conditions, compounds with Papp (A-B)&gt;3 x 10(-6) cm/s have high brain uptake potential; compounds with Papp (A-B)&lt;1 x 10(-6) cm/s are unable to penetrate the blood-brain barrier (BBB); the brain uptake of compounds with Papp (A-B)&lt;1 x 10(-6) cm/s and a P-gp-mediated efflux ratio of &gt;100 may be enhanced by inhibiting P-gp</t>
+  </si>
+  <si>
+    <t>We propose the formulation and characterization of solid microparticles as nasal drug delivery systems able to increase the nose-to-brain transport of deferoxamine mesylate (DFO), a neuroprotector unable to cross the blood brain barrier and inducing negative peripheral impacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> However, this drug does not cross the blood-brain barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Intracerebral implantation of engineered cells encapsulated in a semipermeable polymer membrane constitutes one way to deliver bioactive substances unable to cross the blood-brain barrier while avoiding the need for long-term immunosuppression</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Doxorubicin (DOX) and methotrexate (MTX) showed to be effective against a wide range of tumors, but its use in GBM treatment is limited in part due to the inability to cross the blood-brain barrier (BBB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Although the antioxidant ascorbic acid (AA) or vitamin C does not penetrate the blood-brain barrier (BBB), its oxidized form, dehydroascorbic acid (DHA), enters the brain by means of facilitative transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Horseradish peroxidase (HRP, 40 kDa) was chosen as a model drug, since it normally does not cross the blood-brain barrier (BBB) and its concentration in biological media can be easily quantified</t>
+  </si>
+  <si>
+    <t>Loperamide, an opiate receptor agonist, does not cross the blood-brain barrier because it is a substrate for the permeability-glycoprotein (P-gp) efflux pump</t>
+  </si>
+  <si>
+    <t>) which does not cross the blood brain barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Considering that endogenous opioids may also exhibit anti-inflammatory activities in the periphery, we examined the consequences of a peripheral opioid receptor blockade by naloxone-methiodide, a general opioid receptor antagonist unable to cross the blood-brain barrier, on the development of piroxicam-accelerated colitis in IL-10-deficient (IL-10-/-) mice</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Also, AME does not cross the blood-brain barrier appreciably, so that a therapeutic level in blood can be expected without encountering neurotoxicity</t>
   </si>
   <si>
     <t>Ribavirin is a water-soluble antiviral compound which, owing to its inability to cross the blood-brain barrier, has limited effectiveness in treating viruses affecting the central nervous system</t>
   </si>
   <si>
-    <t xml:space="preserve"> Considering that endogenous opioids may also exhibit anti-inflammatory activities in the periphery, we examined the consequences of a peripheral opioid receptor blockade by naloxone-methiodide, a general opioid receptor antagonist unable to cross the blood-brain barrier, on the development of piroxicam-accelerated colitis in IL-10-deficient (IL-10-/-) mice</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> However, being unable to cross the blood-brain barrier (BBB), CNF1 requires injection directly into the brain, which is a very invasive administration route</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3BP does not cross the blood-brain barrier and cannot treat nervous system tumors</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Many of the current therapeutics have limited activity due to their inability to cross the blood brain barrier which retards drug accumulation in tumor site and causes drug resistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> However, their clinical usage is hindered by their inability to cross the blood-brain barrier and their poor in vivo activity after peripheral injection</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Although metal chelators can block these effects, their therapeutic potential is marred by their inability to cross the blood-brain barrier (BBB) and by their non-specific interactions with metal ions necessary for normal cellular processes, which could result in adverse side effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> We conclude that (11)C-dihydroergotamine is unable to cross the blood-brain barrier interictally or ictally demonstrating that the blood-brain barrier remains tight for dihydroergotamine during acute glyceryl trinitrate-induced migraine attacks</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Due to its hydrophilic actions, circulating AngII does not cross the blood-brain barrier (BBB), signalling to the brain via the circumventricular organs which lack a tight BBB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> However, the clinical usage of these peptides is limited because of their diminished analgesic effect following systemic injection and their inability to cross the blood-brain barrier</t>
-  </si>
-  <si>
-    <t>We propose the formulation and characterization of solid microparticles as nasal drug delivery systems able to increase the nose-to-brain transport of deferoxamine mesylate (DFO), a neuroprotector unable to cross the blood brain barrier and inducing negative peripheral impacts</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enzyme replacement therapy with recombinant SGSH does not treat the brain because the enzyme is a large molecule drug that does not cross the blood-brain barrier (BBB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Doxorubicin (DOX) and methotrexate (MTX) showed to be effective against a wide range of tumors, but its use in GBM treatment is limited in part due to the inability to cross the blood-brain barrier (BBB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Agents unable to cross the blood brain barrier can be directly infused into the brain parenchyma or lateral ventricle through implanted cannulas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> However, MKT-077 does not penetrate the blood-brain barrier (BBB), limiting its use as either a clinical candidate or probe for exploring Hsp70 as a drug target in the central nervous system (CNS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> They showed very low permeability through (MDCK-MDR1) cells and might, therefore, represent possible lead structures for further optimization in the search for cannabinoid ligands unable to cross the blood-brain barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MPS-II affects the brain, and enzyme replacement therapy is not effective in the brain, because the enzyme does not cross the blood-brain barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> However, GDNF does not cross the blood-brain barrier (BBB)</t>
-  </si>
-  <si>
-    <t>Loperamide, an opiate receptor agonist, does not cross the blood-brain barrier because it is a substrate for the permeability-glycoprotein (P-gp) efflux pump</t>
-  </si>
-  <si>
-    <t>Despite its inability to cross the blood-brain barrier, amifostine appears promising because it protects blood vessels against radiation-induced damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Under our experimental conditions, compounds with Papp (A-B)&gt;3 x 10(-6) cm/s have high brain uptake potential; compounds with Papp (A-B)&lt;1 x 10(-6) cm/s are unable to penetrate the blood-brain barrier (BBB); the brain uptake of compounds with Papp (A-B)&lt;1 x 10(-6) cm/s and a P-gp-mediated efflux ratio of &gt;100 may be enhanced by inhibiting P-gp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Horseradish peroxidase (HRP, 40 kDa) was chosen as a model drug, since it normally does not cross the blood-brain barrier (BBB) and its concentration in biological media can be easily quantified</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> However, this drug does not cross the blood-brain barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Intracerebral implantation of engineered cells encapsulated in a semipermeable polymer membrane constitutes one way to deliver bioactive substances unable to cross the blood-brain barrier while avoiding the need for long-term immunosuppression</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Although the antioxidant ascorbic acid (AA) or vitamin C does not penetrate the blood-brain barrier (BBB), its oxidized form, dehydroascorbic acid (DHA), enters the brain by means of facilitative transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> On the other hand, both DCKA and DCKA conjugates have a low brain-to-plasma concentration ratio due to their inability to cross the blood-brain barrier (BBB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ascorbic acid was not able to cross the blood-brain barrier in our studies</t>
-  </si>
-  <si>
-    <t>) which does not cross the blood brain barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> As carbachol does not cross the blood-brain barrier (BBB) due to its polar structure the data support the view that grafts of fetal neuronal tissue may induce a prolonged permeability of the BBB over a long period of time which could also be shown by HRP-histochemistry</t>
-  </si>
-  <si>
-    <t>We examined the potential of astemizole, a histamine H1-receptor antagonist that does not cross the blood-brain barrier, to reverse blood-retinal barrier leakage to albumin in streptozotocin diabetic rats</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Also, AME does not cross the blood-brain barrier appreciably, so that a therapeutic level in blood can be expected without encountering neurotoxicity</t>
-  </si>
-  <si>
-    <t>Apraclonidine hydrochloride (ALO 2145), a clonidine derivative that does not cross the blood-brain barrier, was applied topically to one eye of each of 20 normal human subjects</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aspartic acid, which is also considered to be a transmitter, equally does not cross the blood-brain barrier in the rat with ease</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
     <t>Fail</t>
   </si>
   <si>
+    <t>CCS(=O)(=O)N[C@H](CC1=CC=C(C=C1)C2=CC=CC=C2)C(=O)N[C@@H](CCC(=O)N)C(=O)NCC3=CC=C(C=C3)C(=N)N</t>
+  </si>
+  <si>
+    <t>C(CN)CNCCSP(=O)(O)O</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>C1CN=C(N1)NC2=C(C=C(C=C2Cl)N)Cl.Cl</t>
+  </si>
+  <si>
+    <t>C([C@@H]([C@@H]1C(=C(C(=O)O1)O)O)O)O</t>
+  </si>
+  <si>
+    <t>C([C@@H](C(=O)O)N)C(=O)O</t>
+  </si>
+  <si>
+    <t>COC1=CC=C(C=C1)CCN2CCC(CC2)NC3=NC4=CC=CC=C4N3CC5=CC=C(C=C5)F</t>
+  </si>
+  <si>
+    <t>C[N+](C)(C)CCOC(=O)N.[Cl-]</t>
+  </si>
+  <si>
+    <t>CC(=O)N(CCCCCNC(=O)CCC(=O)N(CCCCCNC(=O)CCC(=O)N(CCCCCN)O)O)O.CS(=O)(=O)O</t>
+  </si>
+  <si>
+    <t>C[C@H]1[C@H]([C@H](C[C@@H](O1)O[C@H]2C[C@@](CC3=C2C(=C4C(=C3O)C(=O)C5=C(C4=O)C(=CC=C5)OC)O)(C(=O)CO)O)N)O</t>
+  </si>
+  <si>
+    <t>C1=CC=C(C(=C1)N)NC(=O)C2=CC=C(C=C2)CNC3=NC=CC(=N3)C4=CN=CC=C4</t>
+  </si>
+  <si>
+    <t>CN(C)C(=O)C(CCN1CCC(CC1)(C2=CC=C(C=C2)Cl)O)(C3=CC=CC=C3)C4=CC=CC=C4</t>
+  </si>
+  <si>
+    <t>CN(CC1=CN=C2C(=N1)C(=NC(=N2)N)N)C3=CC=C(C=C3)C(=O)N[C@@H](CCC(=O)O)C(=O)O</t>
+  </si>
+  <si>
+    <t>C[N+]1(CC[C@]23[C@@H]4C(=O)CC[C@]2([C@H]1CC5=C3C(=C(C=C5)O)O4)O)CC=C.[I-]</t>
+  </si>
+  <si>
     <t>C1=NC(=NN1[C@H]2[C@@H]([C@@H]([C@H](O2)CO)O)O)C(=O)N</t>
   </si>
   <si>
-    <t>C[N+]1(CC[C@]23[C@@H]4C(=O)CC[C@]2([C@H]1CC5=C3C(=C(C=C5)O)O4)O)CC=C.[I-]</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>CCS(=O)(=O)N[C@H](CC1=CC=C(C=C1)C2=CC=CC=C2)C(=O)N[C@@H](CCC(=O)N)C(=O)NCC3=CC=C(C=C3)C(=N)N</t>
-  </si>
-  <si>
-    <t>CC(=O)N(CCCCCNC(=O)CCC(=O)N(CCCCCNC(=O)CCC(=O)N(CCCCCN)O)O)O.CS(=O)(=O)O</t>
-  </si>
-  <si>
-    <t>C[C@H]1[C@H]([C@H](C[C@@H](O1)O[C@H]2C[C@@](CC3=C2C(=C4C(=C3O)C(=O)C5=C(C4=O)C(=CC=C5)OC)O)(C(=O)CO)O)N)O</t>
-  </si>
-  <si>
-    <t>CN(CC1=CN=C2C(=N1)C(=NC(=N2)N)N)C3=CC=C(C=C3)C(=O)N[C@@H](CCC(=O)O)C(=O)O</t>
-  </si>
-  <si>
-    <t>CN(C)C(=O)C(CCN1CCC(CC1)(C2=CC=C(C=C2)Cl)O)(C3=CC=CC=C3)C4=CC=CC=C4</t>
-  </si>
-  <si>
-    <t>C(CN)CNCCSP(=O)(O)O</t>
-  </si>
-  <si>
-    <t>C1=CC=C(C(=C1)N)NC(=O)C2=CC=C(C=C2)CNC3=NC=CC(=N3)C4=CN=CC=C4</t>
-  </si>
-  <si>
     <t>C([C@@H]([C@@H]1C(=O)C(=O)C(=O)O1)O)O</t>
   </si>
   <si>
-    <t>C1=C(C=C(C2=C1NC(=CC2=O)C(=O)O)Cl)Cl</t>
-  </si>
-  <si>
-    <t>C([C@@H]([C@@H]1C(=C(C(=O)O1)O)O)O)O</t>
-  </si>
-  <si>
-    <t>C[N+](C)(C)CCOC(=O)N.[Cl-]</t>
-  </si>
-  <si>
-    <t>COC1=CC=C(C=C1)CCN2CCC(CC2)NC3=NC4=CC=CC=C4N3CC5=CC=C(C=C5)F</t>
-  </si>
-  <si>
-    <t>C1CN=C(N1)NC2=C(C=C(C=C2Cl)N)Cl.Cl</t>
-  </si>
-  <si>
-    <t>C([C@@H](C(=O)O)N)C(=O)O</t>
+    <t>3BP</t>
+  </si>
+  <si>
+    <t>amifostine</t>
+  </si>
+  <si>
+    <t>CNF1</t>
+  </si>
+  <si>
+    <t>Apraclonidine hydrochloride</t>
+  </si>
+  <si>
+    <t>(11)C-dihydroergotamine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AngII</t>
+  </si>
+  <si>
+    <t>Ascorbic acid</t>
+  </si>
+  <si>
+    <t>Aspartic acid</t>
+  </si>
+  <si>
+    <t>astemizole</t>
+  </si>
+  <si>
+    <t>MKT-077</t>
+  </si>
+  <si>
+    <t>GDNF</t>
+  </si>
+  <si>
+    <t>carbachol</t>
+  </si>
+  <si>
+    <t>DCKA</t>
+  </si>
+  <si>
+    <t>deferoxamine mesylate</t>
+  </si>
+  <si>
+    <t>Doxorubicin</t>
+  </si>
+  <si>
+    <t>antioxidant ascorbic acid</t>
+  </si>
+  <si>
+    <t>Horseradish peroxidase</t>
+  </si>
+  <si>
+    <t>Loperamide</t>
+  </si>
+  <si>
+    <t>methotrexate</t>
+  </si>
+  <si>
+    <t>naloxone-methiodide</t>
+  </si>
+  <si>
+    <t>AME</t>
   </si>
   <si>
     <t>Ribavirin</t>
   </si>
   <si>
-    <t>naloxone-methiodide</t>
-  </si>
-  <si>
-    <t>CNF1</t>
-  </si>
-  <si>
-    <t>3BP</t>
-  </si>
-  <si>
-    <t>(11)C-dihydroergotamine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AngII</t>
-  </si>
-  <si>
-    <t>deferoxamine mesylate</t>
-  </si>
-  <si>
-    <t>Doxorubicin</t>
-  </si>
-  <si>
-    <t>methotrexate</t>
-  </si>
-  <si>
-    <t>MKT-077</t>
-  </si>
-  <si>
-    <t>GDNF</t>
-  </si>
-  <si>
-    <t>Loperamide</t>
-  </si>
-  <si>
-    <t>amifostine</t>
-  </si>
-  <si>
-    <t>Horseradish peroxidase</t>
-  </si>
-  <si>
     <t>dehydroascorbic acid</t>
-  </si>
-  <si>
-    <t>antioxidant ascorbic acid</t>
-  </si>
-  <si>
-    <t>DCKA</t>
-  </si>
-  <si>
-    <t>Ascorbic acid</t>
-  </si>
-  <si>
-    <t>carbachol</t>
-  </si>
-  <si>
-    <t>astemizole</t>
-  </si>
-  <si>
-    <t>AME</t>
-  </si>
-  <si>
-    <t>Apraclonidine hydrochloride</t>
-  </si>
-  <si>
-    <t>Aspartic acid</t>
-  </si>
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>blood brain barrier permeability</t>
   </si>
 </sst>
 </file>
@@ -824,20 +821,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" customWidth="1"/>
-    <col min="6" max="6" width="58.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="40.88671875" customWidth="1"/>
+    <col min="6" max="6" width="58.77734375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="14.77734375" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -851,25 +848,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -877,28 +874,28 @@
         <v>30154655</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -909,60 +906,60 @@
         <v>15736415</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>32375387</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -973,199 +970,199 @@
         <v>3062536</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="I5" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>29597041</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>28732166</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="72" hidden="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>27619837</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>27234268</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>26580484</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>57</v>
+      <c r="F10" t="s">
+        <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>26116761</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1173,57 +1170,57 @@
         <v>9389750</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I12" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>24949884</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>60</v>
+      <c r="F13" t="s">
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1231,28 +1228,28 @@
         <v>17948</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H14" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="I14" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1263,141 +1260,141 @@
         <v>1482780</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H15" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I15" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>23931595</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>62</v>
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>23472668</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>63</v>
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>23085772</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>64</v>
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>22065691</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>65</v>
+      <c r="F19" t="s">
+        <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -1405,121 +1402,121 @@
         <v>21502195</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E20" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>66</v>
+      <c r="F20" t="s">
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7755900</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I21" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>11378521</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>74</v>
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H22" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>15620875</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>69</v>
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>72</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -1527,28 +1524,28 @@
         <v>25620068</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I24" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1559,144 +1556,144 @@
         <v>12871659</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>71</v>
+      <c r="F25" t="s">
+        <v>74</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12787846</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>72</v>
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>75</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>11573006</v>
+        <v>24652521</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I27" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>11573006</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>73</v>
+        <v>49</v>
+      </c>
+      <c r="F28" t="s">
+        <v>77</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>24652521</v>
+        <v>15203893</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="G29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H29" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="I29" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -1704,31 +1701,31 @@
     </row>
     <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>15203893</v>
+        <v>18344435</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
         <v>45</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="G30" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="I30" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -1739,185 +1736,185 @@
         <v>8825349</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>24652521</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G31" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>18344435</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="G32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H32" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="I32" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>24652521</v>
+        <v>34299013</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G33" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H33" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="I33" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="J33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2386367</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>79</v>
+      <c r="F34" t="s">
+        <v>82</v>
       </c>
       <c r="G34" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I34" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>34299013</v>
+        <v>34452087</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="G35" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H35" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="I35" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="J35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>34452087</v>
+        <v>11573006</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="G36" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H36" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="I36" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1936,7 +1933,6 @@
         <filter val="C[C@H]1[C@H]([C@H](C[C@@H](O1)O[C@H]2C[C@@](CC3=C2C(=C4C(=C3O)C(=O)C5=C(C4=O)C(=CC=C5)OC)O)(C(=O)CO)O)N)O"/>
         <filter val="C[N+](C)(C)CCOC(=O)N.[Cl-]"/>
         <filter val="C[N+]1(CC[C@]23[C@@H]4C(=O)CC[C@]2([C@H]1CC5=C3C(=C(C=C5)O)O4)O)CC=C.[I-]"/>
-        <filter val="C1=C(C=C(C2=C1NC(=CC2=O)C(=O)O)Cl)Cl"/>
         <filter val="C1=CC=C(C(=C1)N)NC(=O)C2=CC=C(C=C2)CNC3=NC=CC(=N3)C4=CN=CC=C4"/>
         <filter val="C1=NC(=NN1[C@H]2[C@@H]([C@@H]([C@H](O2)CO)O)O)C(=O)N"/>
         <filter val="C1CN=C(N1)NC2=C(C=C(C=C2Cl)N)Cl.Cl"/>
@@ -1948,47 +1944,46 @@
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J36">
-      <sortCondition ref="I1:I36"/>
+      <sortCondition ref="J1:J36"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B35" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B24" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B29" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B33" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B32" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B3" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B30" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B22" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B12" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B21" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B15" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B5" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B14" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>